<commit_message>
add feature values and their means + only flagged survey in univariate
</commit_message>
<xml_diff>
--- a/conf/base/variable_map_explanation.xlsx
+++ b/conf/base/variable_map_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francesco.gizzarelli\Desktop\PoC\audit_anomaly_detection_ETL\conf\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68096D28-EB75-40BC-803A-555326D74E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133E601F-5041-4582-9DD5-A268F8493867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,18 +59,12 @@
     <t>Identifier</t>
   </si>
   <si>
-    <t>This is the unique identifier for the survey.</t>
-  </si>
-  <si>
     <t>enum_id</t>
   </si>
   <si>
     <t>Enumerator ID</t>
   </si>
   <si>
-    <t>This identifies the enumerator responsible for the survey.</t>
-  </si>
-  <si>
     <t>anomaly_prediction</t>
   </si>
   <si>
@@ -80,18 +74,12 @@
     <t>Anomaly Detection</t>
   </si>
   <si>
-    <t>This indicates whether an anomaly has been detected in the survey data.</t>
-  </si>
-  <si>
     <t>anomaly_score</t>
   </si>
   <si>
     <t>Anomaly score</t>
   </si>
   <si>
-    <t>This score reflects the severity of the detected anomaly.</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
@@ -101,9 +89,6 @@
     <t>Time Overall</t>
   </si>
   <si>
-    <t>This represents the total time taken to complete the survey.</t>
-  </si>
-  <si>
     <t>duration_minimum_outlier</t>
   </si>
   <si>
@@ -113,63 +98,42 @@
     <t>Data Quality</t>
   </si>
   <si>
-    <t>This flag indicates if the survey duration is unusually short.</t>
-  </si>
-  <si>
     <t>num_questions</t>
   </si>
   <si>
     <t>Number of survey questions</t>
   </si>
   <si>
-    <t>This shows the total number of questions in the survey.</t>
-  </si>
-  <si>
     <t>time_per_question</t>
   </si>
   <si>
     <t>Average time per question</t>
   </si>
   <si>
-    <t>This is the average time spent on each question in the survey.</t>
-  </si>
-  <si>
     <t>notin_daytime</t>
   </si>
   <si>
     <t>Not initialized during working day flag</t>
   </si>
   <si>
-    <t>This flag indicates whether the survey was initiated outside normal working hours.</t>
-  </si>
-  <si>
     <t>largest_relative_pace_increase</t>
   </si>
   <si>
     <t>Largest relative increase in median pace</t>
   </si>
   <si>
-    <t>This measures the largest relative increase in median pace during the survey.</t>
-  </si>
-  <si>
     <t>nb_value_modifications</t>
   </si>
   <si>
     <t>Number of Value Modifications in the Survey</t>
   </si>
   <si>
-    <t>This counts how many times values were modified in the survey.</t>
-  </si>
-  <si>
     <t>resume_count</t>
   </si>
   <si>
     <t>Number of Survey Resumes</t>
   </si>
   <si>
-    <t>This indicates how many times the survey was resumed.</t>
-  </si>
-  <si>
     <t>constraint_note_count</t>
   </si>
   <si>
@@ -179,27 +143,18 @@
     <t>Kobo Constraint</t>
   </si>
   <si>
-    <t>This counts the number of constraints that were triggered during the survey.</t>
-  </si>
-  <si>
     <t>constraint_backtracks_count</t>
   </si>
   <si>
     <t>Number of Backtracks in Constraints</t>
   </si>
   <si>
-    <t>This counts how many times there were backtracks in constraint validation.</t>
-  </si>
-  <si>
     <t>constraint_error_count</t>
   </si>
   <si>
     <t>Number of Triggered Errors</t>
   </si>
   <si>
-    <t>This indicates the total number of errors triggered during the survey.</t>
-  </si>
-  <si>
     <t>mean_event_time_difference</t>
   </si>
   <si>
@@ -209,88 +164,133 @@
     <t>Time Comparaison</t>
   </si>
   <si>
-    <t>This reflects the average deviation of time spent for each question.</t>
-  </si>
-  <si>
     <t>median_event_time_difference</t>
   </si>
   <si>
     <t>Median time deviation per question</t>
   </si>
   <si>
-    <t>This indicates the median deviation of time spent for each question.</t>
-  </si>
-  <si>
     <t>std_event_time_difference</t>
   </si>
   <si>
     <t>Standard deviation of time per question</t>
   </si>
   <si>
-    <t>This represents the variability in time taken for each question.</t>
-  </si>
-  <si>
     <t>mean_median_difference_event_time_difference</t>
   </si>
   <si>
     <t>Difference between average and median time deviation</t>
   </si>
   <si>
-    <t>This shows the difference between average and median time deviations for questions.</t>
-  </si>
-  <si>
     <t>mean_event_time_difference_group_question</t>
   </si>
   <si>
     <t>Average time deviation per question group</t>
   </si>
   <si>
-    <t>This indicates the average time deviation for questions within a group of questions.</t>
-  </si>
-  <si>
     <t>median_event_time_difference_group_question</t>
   </si>
   <si>
     <t>Median time deviation per question group</t>
   </si>
   <si>
-    <t>This reflects the median time deviation for questions within a group of questions.</t>
-  </si>
-  <si>
     <t>std_event_time_difference_group_question</t>
   </si>
   <si>
     <t>Standard deviation of time per question group</t>
   </si>
   <si>
-    <t>This measures the variability of time for questions within a group of questions.</t>
-  </si>
-  <si>
     <t>mean_median_difference_time_difference_group_question</t>
   </si>
   <si>
     <t>Difference between average and median time deviation for question group</t>
   </si>
   <si>
-    <t>This indicates the difference between average and median time deviations for a group of questions.</t>
-  </si>
-  <si>
     <t>nb_event_time_outside_1_5_IQR</t>
   </si>
   <si>
     <t>Number of quantile outliers</t>
   </si>
   <si>
-    <t>This counts the number of outliers identified based on quantiles (1.5 quantile interval).</t>
-  </si>
-  <si>
     <t>nb_event_time_outside_delta_std</t>
   </si>
   <si>
     <t>Number of standard deviation outliers</t>
   </si>
   <si>
-    <t>This counts the number of outliers identified based on standard deviation (2 sigma).</t>
+    <t>This is the unique identifier for the survey</t>
+  </si>
+  <si>
+    <t>This identifies the enumerator responsible for the survey</t>
+  </si>
+  <si>
+    <t>This indicates whether an anomaly has been detected in the survey data</t>
+  </si>
+  <si>
+    <t>This score reflects the severity of the detected anomaly</t>
+  </si>
+  <si>
+    <t>This represents the total time taken to complete the survey</t>
+  </si>
+  <si>
+    <t>This flag indicates if the survey duration is unusually short</t>
+  </si>
+  <si>
+    <t>This shows the total number of questions in the survey</t>
+  </si>
+  <si>
+    <t>This is the average time spent on each question in the survey</t>
+  </si>
+  <si>
+    <t>This flag indicates whether the survey was initiated outside normal working hours</t>
+  </si>
+  <si>
+    <t>This measures the largest relative increase in median pace during the survey</t>
+  </si>
+  <si>
+    <t>This counts how many times values were modified in the survey</t>
+  </si>
+  <si>
+    <t>This indicates how many times the survey was resumed</t>
+  </si>
+  <si>
+    <t>This counts the number of constraints that were triggered during the survey</t>
+  </si>
+  <si>
+    <t>This counts how many times there were backtracks in constraint validation</t>
+  </si>
+  <si>
+    <t>This indicates the total number of errors triggered during the survey</t>
+  </si>
+  <si>
+    <t>This reflects the average deviation of time spent for each question</t>
+  </si>
+  <si>
+    <t>This indicates the median deviation of time spent for each question</t>
+  </si>
+  <si>
+    <t>This represents the variability in time taken for each question</t>
+  </si>
+  <si>
+    <t>This shows the difference between average and median time deviations for questions</t>
+  </si>
+  <si>
+    <t>This indicates the average time deviation for questions within a group of questions</t>
+  </si>
+  <si>
+    <t>This reflects the median time deviation for questions within a group of questions</t>
+  </si>
+  <si>
+    <t>This measures the variability of time for questions within a group of questions</t>
+  </si>
+  <si>
+    <t>This indicates the difference between average and median time deviations for a group of questions</t>
+  </si>
+  <si>
+    <t>This counts the number of outliers identified based on quantiles (1.5 quantile interval)</t>
+  </si>
+  <si>
+    <t>This counts the number of outliers identified based on standard deviation (2 sigma)</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="78.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -743,340 +745,340 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>84</v>
@@ -1088,6 +1090,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE51FB2AFBB2DD429D3D11FE759FFC43" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="8d091c5c4a4a813be39ea735a73ac9df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f4877444-78fa-4cfa-bafc-d6c64fafc061" xmlns:ns3="d0fa6634-326e-4532-91a2-52bea7ac9212" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9faba7501e101522608015841357ce76" ns2:_="" ns3:_="">
     <xsd:import namespace="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
@@ -1316,27 +1338,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4D81FC1-7373-4393-AF88-2295169327F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
+    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276E393F-A186-4F48-B78F-24839AA9B19D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE929793-99A1-445A-AA8C-A57131B06D6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1353,23 +1374,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276E393F-A186-4F48-B78F-24839AA9B19D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4D81FC1-7373-4393-AF88-2295169327F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
-    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>